<commit_message>
Added some diagnostic plots to AnalysisBr_nearline.C, needs serious tidying
</commit_message>
<xml_diff>
--- a/RadialFieldOps_2/RadialFieldScan.xlsx
+++ b/RadialFieldOps_2/RadialFieldScan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/RadialFieldOps_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A01643-28B5-9941-B868-B36852F4C1F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E27F184-4D77-5648-B502-B80939CAEAC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="460" windowWidth="32120" windowHeight="17540" xr2:uid="{3DAFEA06-3AA8-BB44-8E27-DDA65B3686C5}"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="32120" windowHeight="17540" activeTab="3" xr2:uid="{3DAFEA06-3AA8-BB44-8E27-DDA65B3686C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3983,10 +3983,10 @@
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4313,8 +4313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B752E6E-F960-2F47-AC55-2B0104D935A3}">
   <dimension ref="A2:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="65" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="Y35" sqref="Y30:Z35"/>
+    <sheetView zoomScale="65" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5335,6 +5335,12 @@
         <v>2049274</v>
       </c>
     </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J39" s="1">
+        <f>AVERAGE(J4:J9,J13:J18,J22:J27,J31:J36)</f>
+        <v>2230435.5416666665</v>
+      </c>
+    </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
@@ -5370,7 +5376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF6A8D8-01A0-1C46-A2D1-628E1D9A77A8}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="Q25" sqref="Q2:S25"/>
     </sheetView>
   </sheetViews>
@@ -6549,7 +6555,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6643,20 +6649,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419E4AC4-5F94-BA40-832F-928FA2C4F999}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -6667,7 +6673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6677,10 +6683,38 @@
       <c r="C4">
         <v>37886</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>37885</v>
+      </c>
+      <c r="G5">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="H5">
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <f>ABS(G4-G5)</f>
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="H6">
+        <f>SQRT(H5^2)</f>
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <f>G6/H6</f>
+        <v>0.29673202614379085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made proper effort to fit the vertical COD
</commit_message>
<xml_diff>
--- a/RadialFieldOps_2/RadialFieldScan.xlsx
+++ b/RadialFieldOps_2/RadialFieldScan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/RadialFieldOps_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E27F184-4D77-5648-B502-B80939CAEAC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D8D0A1-880D-5645-A145-0C5F1CE78E4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="460" windowWidth="32120" windowHeight="17540" activeTab="3" xr2:uid="{3DAFEA06-3AA8-BB44-8E27-DDA65B3686C5}"/>
+    <workbookView xWindow="780" yWindow="-19340" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{3DAFEA06-3AA8-BB44-8E27-DDA65B3686C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6652,7 +6652,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B5" sqref="B4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>